<commit_message>
Arrumando bugs e adicionando media da classe
</commit_message>
<xml_diff>
--- a/assets/spreadsheets/Modelo de Gabarito Street Fighter.xlsx
+++ b/assets/spreadsheets/Modelo de Gabarito Street Fighter.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinim\Documents\Projects GitHub\Automated-Multiple-Choice-Exam-Grading-System\assets\spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinim\Documents\Projects GitHub\Corretor-Expresso\assets\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C7027DB-48DB-4EF2-BD6B-DA7C1EC49552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FBB689B-1C61-4A59-A3AD-1BCF45D04DAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{D3219A13-647C-4E61-9BEB-CAC4A9BE4460}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D3219A13-647C-4E61-9BEB-CAC4A9BE4460}"/>
   </bookViews>
   <sheets>
     <sheet name="Mulheres" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="82">
   <si>
     <t>NUMERO DA QUESTÃO</t>
   </si>
@@ -277,6 +277,12 @@
   </si>
   <si>
     <t>Street Fighter Feminino</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>FIT</t>
   </si>
 </sst>
 </file>
@@ -448,7 +454,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -476,9 +482,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -490,50 +493,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="41">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="5" tint="-0.24994659260841701"/>
-          <bgColor rgb="FFFFFF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor theme="1"/>
-          <bgColor theme="3" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -769,6 +728,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
@@ -776,7 +742,44 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor theme="5" tint="-0.24994659260841701"/>
+          <bgColor rgb="FFFFFF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor theme="1"/>
+          <bgColor theme="3" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1142,44 +1145,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48AAFFEA-A9E9-4C5A-8CE0-EA7E7C4F864F}">
   <dimension ref="A1:X20"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:F3"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA13" sqref="AA13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="11" width="3.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="23" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="11" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="24" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
-      <c r="W1" s="13"/>
-      <c r="X1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12"/>
     </row>
     <row r="2" spans="1:24" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -1251,6 +1253,9 @@
       <c r="W2" s="4" t="s">
         <v>76</v>
       </c>
+      <c r="X2" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="3" spans="1:24" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
@@ -1322,6 +1327,9 @@
       <c r="W3" s="4" t="s">
         <v>49</v>
       </c>
+      <c r="X3" s="4" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="4" spans="1:24" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
@@ -1393,6 +1401,9 @@
       <c r="W4" s="6" t="s">
         <v>50</v>
       </c>
+      <c r="X4" s="6" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="5" spans="1:24" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
@@ -1464,6 +1475,9 @@
       <c r="W5" s="6" t="s">
         <v>50</v>
       </c>
+      <c r="X5" s="6" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="6" spans="1:24" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
@@ -1535,6 +1549,9 @@
       <c r="W6" s="6" t="s">
         <v>27</v>
       </c>
+      <c r="X6" s="6" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="7" spans="1:24" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
@@ -1606,6 +1623,9 @@
       <c r="W7" s="6" t="s">
         <v>28</v>
       </c>
+      <c r="X7" s="6" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="8" spans="1:24" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
@@ -1677,6 +1697,9 @@
       <c r="W8" s="6" t="s">
         <v>50</v>
       </c>
+      <c r="X8" s="6" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="9" spans="1:24" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
@@ -1748,6 +1771,9 @@
       <c r="W9" s="6" t="s">
         <v>28</v>
       </c>
+      <c r="X9" s="6" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="10" spans="1:24" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
@@ -1819,6 +1845,9 @@
       <c r="W10" s="6" t="s">
         <v>50</v>
       </c>
+      <c r="X10" s="6" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="11" spans="1:24" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
@@ -1888,6 +1917,9 @@
       <c r="W11" s="6" t="s">
         <v>28</v>
       </c>
+      <c r="X11" s="6" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="12" spans="1:24" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
@@ -1959,6 +1991,9 @@
       <c r="W12" s="6" t="s">
         <v>50</v>
       </c>
+      <c r="X12" s="6" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="13" spans="1:24" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
@@ -2027,6 +2062,9 @@
       </c>
       <c r="W13" s="6" t="s">
         <v>28</v>
+      </c>
+      <c r="X13" s="6" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:24" ht="16.2" x14ac:dyDescent="0.35">
@@ -2055,6 +2093,9 @@
       <c r="U14" s="6"/>
       <c r="V14" s="6"/>
       <c r="W14" s="6"/>
+      <c r="X14" s="6" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="15" spans="1:24" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
@@ -2126,6 +2167,9 @@
       <c r="W15" s="6" t="s">
         <v>28</v>
       </c>
+      <c r="X15" s="6" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="16" spans="1:24" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A16" s="9" t="s">
@@ -2197,8 +2241,11 @@
       <c r="W16" s="6" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="17" spans="1:23" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="X16" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
         <v>43</v>
       </c>
@@ -2268,8 +2315,11 @@
       <c r="W17" s="6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="18" spans="1:23" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="X17" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A18" s="9" t="s">
         <v>44</v>
       </c>
@@ -2337,8 +2387,11 @@
       <c r="W18" s="6" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="19" spans="1:23" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="X18" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
         <v>45</v>
       </c>
@@ -2408,8 +2461,11 @@
       <c r="W19" s="6" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="20" spans="1:23" ht="16.2" x14ac:dyDescent="0.35">
+      <c r="X19" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" ht="16.2" x14ac:dyDescent="0.35">
       <c r="A20" s="10" t="s">
         <v>46</v>
       </c>
@@ -2464,7 +2520,7 @@
       <c r="R20" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="S20" s="7" t="s">
+      <c r="S20" s="1" t="s">
         <v>28</v>
       </c>
       <c r="T20" s="8" t="s">
@@ -2477,6 +2533,9 @@
         <v>50</v>
       </c>
       <c r="W20" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="X20" s="6" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2485,27 +2544,27 @@
     <mergeCell ref="A1:W1"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="A3 A4:W20">
-    <cfRule type="expression" dxfId="5" priority="5">
+  <conditionalFormatting sqref="A3 A4:X20">
+    <cfRule type="expression" dxfId="39" priority="5">
       <formula>AND((A3=A$4), (LEN(A3)&lt;2))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="expression" dxfId="38" priority="6">
       <formula>AND((A3&lt;&gt;A$4), (LEN(A3)&lt;2))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:W2">
-    <cfRule type="expression" dxfId="3" priority="2">
+  <conditionalFormatting sqref="A2:X2">
+    <cfRule type="expression" dxfId="37" priority="2">
       <formula>ROW()=2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:W20">
-    <cfRule type="expression" dxfId="2" priority="1">
+  <conditionalFormatting sqref="A3:X20">
+    <cfRule type="expression" dxfId="36" priority="1">
       <formula>ROW()=4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="35" priority="3">
       <formula>$A3="MATÉRIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="4">
+    <cfRule type="expression" dxfId="34" priority="4">
       <formula>AND((A3=""), (LEN(A3)&lt;2))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2517,8 +2576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACB4EE8E-BE0D-4F84-BE74-F980EF0551FE}">
   <dimension ref="A1:U27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3:U3"/>
+    <sheetView topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S27" sqref="S27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2529,29 +2588,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="22.8" x14ac:dyDescent="0.5">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
     </row>
     <row r="2" spans="1:21" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -2749,7 +2808,7 @@
       </c>
     </row>
     <row r="5" spans="1:21" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="11" t="s">
         <v>51</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -2814,7 +2873,7 @@
       </c>
     </row>
     <row r="6" spans="1:21" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="11" t="s">
         <v>52</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -2875,11 +2934,11 @@
         <v>28</v>
       </c>
       <c r="U6" s="6" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="11" t="s">
         <v>53</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -2940,11 +2999,11 @@
         <v>28</v>
       </c>
       <c r="U7" s="6" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="11" t="s">
         <v>54</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -3002,12 +3061,14 @@
         <v>28</v>
       </c>
       <c r="T8" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="U8" s="6"/>
+        <v>28</v>
+      </c>
+      <c r="U8" s="6" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="9" spans="1:21" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="11" t="s">
         <v>55</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -3065,14 +3126,14 @@
         <v>28</v>
       </c>
       <c r="T9" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="U9" s="6" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="11" t="s">
         <v>56</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -3135,7 +3196,7 @@
       </c>
     </row>
     <row r="11" spans="1:21" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="11" t="s">
         <v>57</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -3192,15 +3253,15 @@
       <c r="S11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="T11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="U11" s="1" t="s">
-        <v>28</v>
+      <c r="T11" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="U11" s="6" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="11" t="s">
         <v>58</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -3257,13 +3318,15 @@
       <c r="S12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="T12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="U12" s="1"/>
+      <c r="T12" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="U12" s="6" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="13" spans="1:21" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="11" t="s">
         <v>59</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -3320,15 +3383,15 @@
       <c r="S13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="T13" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="U13" s="7" t="s">
-        <v>28</v>
+      <c r="T13" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="U13" s="6" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="11" t="s">
         <v>68</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -3393,7 +3456,7 @@
       </c>
     </row>
     <row r="15" spans="1:21" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="11" t="s">
         <v>60</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -3452,11 +3515,11 @@
         <v>28</v>
       </c>
       <c r="U15" s="6" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="11" t="s">
         <v>77</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -3512,14 +3575,14 @@
         <v>28</v>
       </c>
       <c r="T16" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="U16" s="6" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="11" t="s">
         <v>61</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -3577,14 +3640,14 @@
         <v>28</v>
       </c>
       <c r="T17" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="U17" s="6" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="11" t="s">
         <v>62</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -3642,12 +3705,14 @@
         <v>28</v>
       </c>
       <c r="T18" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="U18" s="6"/>
+        <v>28</v>
+      </c>
+      <c r="U18" s="6" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="19" spans="1:21" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="11" t="s">
         <v>70</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -3705,14 +3770,14 @@
         <v>28</v>
       </c>
       <c r="T19" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="U19" s="6" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="11" t="s">
         <v>63</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -3766,18 +3831,18 @@
       <c r="R20" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="S20" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="T20" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="U20" s="8" t="s">
+      <c r="S20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="T20" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="U20" s="6" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A21" s="12" t="s">
+      <c r="A21" s="11" t="s">
         <v>71</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -3834,15 +3899,15 @@
       <c r="S21" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="T21" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="U21" s="1" t="s">
-        <v>28</v>
+      <c r="T21" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="U21" s="6" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="11" t="s">
         <v>64</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -3871,15 +3936,15 @@
       <c r="S22" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="T22" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="U22" s="1" t="s">
-        <v>28</v>
+      <c r="T22" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="U22" s="6" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:21" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="11" t="s">
         <v>69</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -3933,18 +3998,18 @@
       <c r="R23" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="S23" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="T23" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="U23" s="7" t="s">
-        <v>28</v>
+      <c r="S23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="T23" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="U23" s="6" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A24" s="12" t="s">
+      <c r="A24" s="11" t="s">
         <v>65</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -3999,17 +4064,17 @@
         <v>29</v>
       </c>
       <c r="S24" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="T24" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="U24" s="1" t="s">
-        <v>28</v>
+        <v>28</v>
+      </c>
+      <c r="T24" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="U24" s="6" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:21" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="11" t="s">
         <v>72</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -4033,12 +4098,18 @@
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
-      <c r="S25" s="1"/>
-      <c r="T25" s="1"/>
-      <c r="U25" s="1"/>
+      <c r="S25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="T25" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="U25" s="6" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="26" spans="1:21" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="11" t="s">
         <v>66</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -4093,17 +4164,17 @@
         <v>29</v>
       </c>
       <c r="S26" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="T26" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="U26" s="7" t="s">
-        <v>28</v>
+        <v>28</v>
+      </c>
+      <c r="T26" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="U26" s="6" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="16.2" x14ac:dyDescent="0.35">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="11" t="s">
         <v>67</v>
       </c>
       <c r="B27" s="7" t="s">
@@ -4158,135 +4229,139 @@
         <v>29</v>
       </c>
       <c r="S27" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="T27" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="U27" s="8"/>
+        <v>28</v>
+      </c>
+      <c r="T27" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="U27" s="6" t="s">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:U1"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="A3 A4:U4 B5:U20 I21:U23 B21:H27 I25:J27">
-    <cfRule type="expression" dxfId="39" priority="56">
-      <formula>AND((A3&lt;&gt;A$4), (LEN(A3)&lt;2))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="38" priority="55">
+  <conditionalFormatting sqref="A3 A4:U4 B6:R20 I21:R23 B21:H27 I25:J27 B5:U5 S6:U27">
+    <cfRule type="expression" dxfId="33" priority="60">
       <formula>AND((A3=A$4), (LEN(A3)&lt;2))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A3 A4:U4 B5:U5 B6:R20 I21:R23 B21:H27 I25:J27 S6:U27">
+    <cfRule type="expression" dxfId="32" priority="61">
+      <formula>AND((A3&lt;&gt;A$4), (LEN(A3)&lt;2))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A5:A27">
-    <cfRule type="expression" dxfId="37" priority="46">
+    <cfRule type="expression" dxfId="31" priority="51">
       <formula>AND((A5=XEE$4), (LEN(A5)&lt;2))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="50">
+    <cfRule type="expression" dxfId="30" priority="55">
       <formula>AND((A5=""), (LEN(A5)&lt;2))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="49">
+    <cfRule type="expression" dxfId="29" priority="54">
       <formula>$AA5="MATÉRIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="48">
+    <cfRule type="expression" dxfId="28" priority="53">
       <formula>ROW()=4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="47">
+    <cfRule type="expression" dxfId="27" priority="52">
       <formula>AND((A5&lt;&gt;XEE$4), (LEN(A5)&lt;2))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:U2">
-    <cfRule type="expression" dxfId="32" priority="52">
+    <cfRule type="expression" dxfId="26" priority="57">
       <formula>ROW()=2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:U4 B6:U20 I21:U23 B21:H27 I25:J27">
-    <cfRule type="expression" dxfId="31" priority="54">
+  <conditionalFormatting sqref="A3:U4 B6:R20 I21:R23 B21:H27 I25:J27">
+    <cfRule type="expression" dxfId="25" priority="59">
       <formula>AND((A3=""), (LEN(A3)&lt;2))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="53">
+    <cfRule type="expression" dxfId="24" priority="58">
       <formula>$A3="MATÉRIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="51">
+    <cfRule type="expression" dxfId="23" priority="56">
       <formula>ROW()=4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B5:U5">
-    <cfRule type="expression" dxfId="28" priority="89">
+  <conditionalFormatting sqref="B5:U5 S6:U27">
+    <cfRule type="expression" dxfId="22" priority="94">
       <formula>AND((B5=""), (LEN(B5)&lt;2))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="88">
+    <cfRule type="expression" dxfId="21" priority="93">
       <formula>$AA5="MATÉRIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="87">
+    <cfRule type="expression" dxfId="20" priority="92">
       <formula>ROW()=4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I24:K24">
-    <cfRule type="expression" dxfId="25" priority="40">
+    <cfRule type="expression" dxfId="19" priority="45">
       <formula>AND((I24&lt;&gt;I$4), (LEN(I24)&lt;2))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="36">
+    <cfRule type="expression" dxfId="18" priority="41">
       <formula>ROW()=4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="37">
+    <cfRule type="expression" dxfId="17" priority="42">
       <formula>$A24="MATÉRIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="38">
+    <cfRule type="expression" dxfId="16" priority="43">
       <formula>AND((I24=""), (LEN(I24)&lt;2))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="39">
+    <cfRule type="expression" dxfId="15" priority="44">
       <formula>AND((I24=I$4), (LEN(I24)&lt;2))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K25:K26">
-    <cfRule type="expression" dxfId="20" priority="25">
+    <cfRule type="expression" dxfId="14" priority="30">
       <formula>AND((K25&lt;&gt;K$4), (LEN(K25)&lt;2))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="24">
+    <cfRule type="expression" dxfId="13" priority="29">
       <formula>AND((K25=K$4), (LEN(K25)&lt;2))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="23">
+    <cfRule type="expression" dxfId="12" priority="28">
       <formula>AND((K25=""), (LEN(K25)&lt;2))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="22">
+    <cfRule type="expression" dxfId="11" priority="27">
       <formula>$A25="MATÉRIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="21">
+    <cfRule type="expression" dxfId="10" priority="26">
       <formula>ROW()=4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K27:U27">
-    <cfRule type="expression" dxfId="15" priority="20">
+  <conditionalFormatting sqref="K27:R27">
+    <cfRule type="expression" dxfId="9" priority="25">
       <formula>AND((K27&lt;&gt;K$4), (LEN(K27)&lt;2))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="19">
+    <cfRule type="expression" dxfId="8" priority="24">
       <formula>AND((K27=K$4), (LEN(K27)&lt;2))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="18">
+    <cfRule type="expression" dxfId="7" priority="23">
       <formula>AND((K27=""), (LEN(K27)&lt;2))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="17">
+    <cfRule type="expression" dxfId="6" priority="22">
       <formula>$A27="MATÉRIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="16">
+    <cfRule type="expression" dxfId="5" priority="21">
       <formula>ROW()=4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L24:U26">
-    <cfRule type="expression" dxfId="10" priority="2">
+  <conditionalFormatting sqref="L24:R26">
+    <cfRule type="expression" dxfId="4" priority="7">
       <formula>$A24="MATÉRIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="5">
+    <cfRule type="expression" dxfId="3" priority="10">
       <formula>AND((L24&lt;&gt;L$4), (LEN(L24)&lt;2))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="4">
+    <cfRule type="expression" dxfId="2" priority="9">
       <formula>AND((L24=L$4), (LEN(L24)&lt;2))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="3">
+    <cfRule type="expression" dxfId="1" priority="8">
       <formula>AND((L24=""), (LEN(L24)&lt;2))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="1">
+    <cfRule type="expression" dxfId="0" priority="6">
       <formula>ROW()=4</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>